<commit_message>
console error bug resolved
</commit_message>
<xml_diff>
--- a/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-kajoll.FAREAST\Desktop\kpi column smaan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\KPIColumn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
     <sheet name="Checklist" sheetId="2" r:id="rId2"/>
+    <sheet name="Bugs-Issues" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
   <si>
     <t>S no</t>
   </si>
@@ -315,20 +316,8 @@
 5. Switch the toggle off</t>
   </si>
   <si>
-    <t>1. Target line's color will be set to 'blue'
-2. If stroke value is '-2' then it will automatically change to '0'
-3. If stroke value is '7' then it will automatically change to '5'
-4. The individual target line should disappear</t>
-  </si>
-  <si>
     <t>1. Dashed line at top of each bar will be displayed signifying target YTD
 2. Target legend will be added in the chart</t>
-  </si>
-  <si>
-    <t>1. Target line's color will be set to 'blue'
-2. If stroke value is '-2' then it will automatically change to '0'
-3. If stroke value is '7' then it will automatically change to '5'
-4. The target line should disappear</t>
   </si>
   <si>
     <t>1. Go to formatting pane
@@ -366,6 +355,122 @@
 3. If bar value is greater than zone 1 upper bound and less than zone 2 upper bound, then 'brown' color will be displayed for bars accordingly
 4. If bar value is greater than zone 2 upper bound, then 'grey' color will be displayed for bars accordingly
 </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Change/ Update visual to make animation appear</t>
+  </si>
+  <si>
+    <t>The columns make transition from the bottom on every update.</t>
+  </si>
+  <si>
+    <t>1. Drag the window or make any other update</t>
+  </si>
+  <si>
+    <t>Adding ToolTip</t>
+  </si>
+  <si>
+    <t>Add a tooltip for additional information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding one or more column to the tooltip bag.  </t>
+  </si>
+  <si>
+    <t>Analytics Functions</t>
+  </si>
+  <si>
+    <t>Min, max, avg and median values appear on the chart</t>
+  </si>
+  <si>
+    <t>Turn on the toggle for one or analytics funciton in the format pane</t>
+  </si>
+  <si>
+    <t>Corresponding horizontal value lines are generated in the chart of max thickness 5 and of any color the user selects.</t>
+  </si>
+  <si>
+    <t>1. The column values are displayed accordingly when mouse is hovered over it.
+2. Adding Multiple similar columns in the bag gives on value in tooltip display: Expected Behaviour. 
+3. If the column added is same as the default tooltip value column, the values are repaeated when mouse if hovered on the columns.</t>
+  </si>
+  <si>
+    <t>S No</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Repro Steps</t>
+  </si>
+  <si>
+    <t>Y-Axis Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Display column lengths as per min and max values specified</t>
+  </si>
+  <si>
+    <t>The length of columns are displayed accordingly.</t>
+  </si>
+  <si>
+    <t>Legend text no aligned properly with legend style for some fonts like Courier New</t>
+  </si>
+  <si>
+    <t>Legend-Title</t>
+  </si>
+  <si>
+    <t>The legend text and type should increase and decrease accordingly</t>
+  </si>
+  <si>
+    <t>Max value of Y-axis start: 2500, can change to any other value manually</t>
+  </si>
+  <si>
+    <t>You can turn the legend title on/off through a toggle and set its size.</t>
+  </si>
+  <si>
+    <t>The browsers IE and Edge lag in increasing/decreasing values manually. On hovering over the legends when the title is turned off, we can see what they stand for.</t>
+  </si>
+  <si>
+    <t>Data Labels are fixed to default value as Y-Axis Start Grid = 2500, should adjust accordingly when the start/end values of the Y-Axis are changed</t>
+  </si>
+  <si>
+    <t>Change default values of Y-Axis start and end, the alignment of Data Labels does not change with the assigned Axis values.</t>
+  </si>
+  <si>
+    <t>In the format pane, select font: courier new, the text is not aligned with the legend style.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The size and color of the target line should change. </t>
+  </si>
+  <si>
+    <t>Turn the toggle on, and set the size to max value of 5 or a min value of 1. And set the color.</t>
+  </si>
+  <si>
+    <t>The thickness and color of the target line and dots changes.</t>
+  </si>
+  <si>
+    <t>Individual Target line and dots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG-Image should be added from the specified url. Turn the toggle funcitonality on and specify the url. </t>
+  </si>
+  <si>
+    <t>Background Image does not span the entire viewport window.</t>
+  </si>
+  <si>
+    <t>1. Target line's color will be set to 'blue'
+2. If stroke value is '-2' then it will automatically change to '1'
+3. If stroke value is '7' then it will automatically change to '5'
+4. The individual target line should disappear</t>
+  </si>
+  <si>
+    <t>1. Target line's color will be set to 'blue'
+2. If stroke value is '-2' then it will automatically change to '1'
+3. If stroke value is '7' then it will automatically change to '5'
+4. The target line should disappear</t>
   </si>
 </sst>
 </file>
@@ -552,6 +657,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2400299</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>657225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A0D36E-1264-4863-BEA2-889E05A4171D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="6086475"/>
+          <a:ext cx="2381249" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>942974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2381250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>2276475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6655B5B8-5F1C-49B0-A4C7-45465CFA686E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="7781924"/>
+          <a:ext cx="2362200" cy="1333501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,9 +1049,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -924,7 +1122,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -958,7 +1156,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -969,7 +1167,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -983,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
@@ -1003,7 +1201,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1020,7 +1218,7 @@
         <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1031,13 +1229,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1055,6 +1253,108 @@
       </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1067,13 +1367,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BDF48F-142E-4DA3-AA46-5DE95B2DDBCD}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="72.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1296,7 +1597,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,14 +1619,14 @@
       <c r="B24" s="12"/>
       <c r="C24" s="18"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="186" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="19"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>19</v>
       </c>
@@ -1355,5 +1656,71 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26582054-7465-4694-8628-66C6584852A7}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bookmark support and UI bug fixes
</commit_message>
<xml_diff>
--- a/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlab\documents\Published\KPIColumn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI-CustomVisuals\documents\Published\KPIColumn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7909B66-CEB9-4193-B3C4-2BE8D7E23072}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABF1E0A-5D72-4F87-8456-02F4F2E4596E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="115">
   <si>
     <t>S no</t>
   </si>
@@ -355,9 +355,6 @@
 </t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Animation</t>
   </si>
   <si>
@@ -472,6 +469,30 @@
   </si>
   <si>
     <t>Update data label's color, text size, display units and decimal value(Max text size is 20)</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Created bookmarks with selection should retain the visual.</t>
+  </si>
+  <si>
+    <t>1.Generate a chart with some data
+2. Go to View and tick the Bookmarks Pane
+3. Perform selections in chart, filter it if you want and save them in different bookmarks using 'update'
+4. Click on the different bookmarks to see them</t>
+  </si>
+  <si>
+    <t>1. Chart will be shown according to the data
+2. The Bookmarks Pane will show up on the right side
+3. According to selections, new bookmarks will be added in the Bookmarks Pane
+4. Based on selections, bookmarks will render visual as saved previously</t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -658,99 +679,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2400299</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>657225</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A0D36E-1264-4863-BEA2-889E05A4171D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5476875" y="6086475"/>
-          <a:ext cx="2381249" cy="1409700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>942974</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2381250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>2276475</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6655B5B8-5F1C-49B0-A4C7-45465CFA686E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5476875" y="7781924"/>
-          <a:ext cx="2362200" cy="1333501"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1051,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1168,7 +1096,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1230,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>69</v>
@@ -1261,16 +1189,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,16 +1206,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1295,16 +1223,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1312,16 +1240,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1329,16 +1257,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="D17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1346,16 +1274,33 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>102</v>
+    </row>
+    <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1368,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BDF48F-142E-4DA3-AA46-5DE95B2DDBCD}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1543,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1602,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1666,7 +1610,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,13 +1621,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1691,10 +1638,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1702,10 +1652,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>98</v>
+      <c r="D3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1713,12 +1666,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
API 2.5 and support for context menu
</commit_message>
<xml_diff>
--- a/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/KPIColumn/KPIColumnByMAQSoftwareChecklist.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\PowerBI-visuals\documents\Published\KPIColumn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\KPIColumn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92A568F-4C20-45D0-8F45-A650A46B02D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F0D6A-DE0D-4847-A6E6-9911F948D069}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="1" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFA628E8-139E-4A70-BE7A-AA996D28E374}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
     <sheet name="Checklist" sheetId="2" r:id="rId2"/>
     <sheet name="Bugs-Issues" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="120">
   <si>
     <t>S no</t>
   </si>
@@ -496,6 +502,20 @@
   </si>
   <si>
     <t>Is report tooltip working properly?</t>
+  </si>
+  <si>
+    <t>Drillthrough</t>
+  </si>
+  <si>
+    <t>Created custom menu to drill through from one visual to another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate a chart with some data
+2.Create new report page and in DrillThrough add the fields for drillthrough.
+3. Right click on the chart, select the Drillthrough option from the menu. </t>
+  </si>
+  <si>
+    <t>1. On right click of the chart and selecting the drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
   </si>
 </sst>
 </file>
@@ -657,16 +677,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -697,34 +713,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1041,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C560CE-405B-4CA8-AB3A-A0EEBCD256B2}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,19 +1086,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1364,6 +1377,23 @@
       </c>
       <c r="E19" s="2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BDF48F-142E-4DA3-AA46-5DE95B2DDBCD}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1387,178 +1417,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1566,7 +1596,7 @@
       <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="19" t="s">
@@ -1575,26 +1605,26 @@
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1602,7 +1632,7 @@
       <c r="A21" s="16">
         <v>18</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -1611,60 +1641,60 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="20"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
-      <c r="B24" s="12"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="20"/>
     </row>
     <row r="25" spans="1:3" ht="186" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="21"/>
     </row>
     <row r="26" spans="1:3" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+      <c r="A26" s="4">
         <v>19</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
+      <c r="A27" s="12">
         <v>20</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="13">
         <v>21</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="15" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>